<commit_message>
changed xxd - 3
</commit_message>
<xml_diff>
--- a/LR3/table_1_4.xlsx
+++ b/LR3/table_1_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38E814DA-7BE8-475A-8A85-F79897097E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD3DCF0-AB77-4776-B247-D6BBA7814AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C812E225-0302-43BC-BF7F-7687DCBD0107}"/>
   </bookViews>
@@ -178,16 +178,16 @@
     <t>Итого, руб.</t>
   </si>
   <si>
-    <t>Общая сумма графы "Итого", руб</t>
-  </si>
-  <si>
-    <t>Средняя площадь, кв.м.</t>
-  </si>
-  <si>
-    <t>Максимальный срок просрочки</t>
-  </si>
-  <si>
-    <t>Максимальная сумма к оплате</t>
+    <t>общая сумма графы "Итого", руб</t>
+  </si>
+  <si>
+    <t>средняя площадь, кв.м.</t>
+  </si>
+  <si>
+    <t>максимальный срок просрочки</t>
+  </si>
+  <si>
+    <t>максимальная сумма к оплате</t>
   </si>
 </sst>
 </file>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F7733E-DEB9-4F9D-8946-67364D2E8DA5}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +647,7 @@
         <v>70</v>
       </c>
       <c r="D3" s="1">
+        <f>4*1.1</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="E3" s="1">
@@ -687,32 +688,33 @@
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
+        <f t="shared" ref="D4:D38" si="0">4*1.1</f>
         <v>4.4000000000000004</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E38" si="0">C4*D4</f>
+        <f t="shared" ref="E4:E38" si="1">C4*D4</f>
         <v>305.8</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:F38" si="1">DATE(2022,9,9)</f>
+        <f t="shared" ref="F4:F38" si="2">DATE(2022,9,9)</f>
         <v>44813</v>
       </c>
       <c r="G4" s="2">
         <v>44806</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H38" si="2">IF(G4&lt;=F4,0,G4-F4)</f>
+        <f t="shared" ref="H4:H38" si="3">IF(G4&lt;=F4,0,G4-F4)</f>
         <v>0</v>
       </c>
       <c r="I4" s="1">
         <v>10</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J38" si="3">I4*H4</f>
+        <f t="shared" ref="J4:J38" si="4">I4*H4</f>
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K38" si="4">E4+J4</f>
+        <f t="shared" ref="K4:K38" si="5">E4+J4</f>
         <v>305.8</v>
       </c>
     </row>
@@ -727,32 +729,33 @@
         <v>69</v>
       </c>
       <c r="D5" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>303.60000000000002</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G5" s="2">
         <v>44807</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I5" s="1">
         <v>10</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>303.60000000000002</v>
       </c>
     </row>
@@ -767,32 +770,33 @@
         <v>68.5</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>301.40000000000003</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G6" s="2">
         <v>44808</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>10</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>301.40000000000003</v>
       </c>
     </row>
@@ -807,32 +811,33 @@
         <v>68</v>
       </c>
       <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>299.20000000000005</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G7" s="2">
         <v>44809</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I7" s="1">
         <v>10</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>299.20000000000005</v>
       </c>
     </row>
@@ -847,32 +852,33 @@
         <v>67.5</v>
       </c>
       <c r="D8" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>297</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G8" s="2">
         <v>44810</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I8" s="1">
         <v>10</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>297</v>
       </c>
     </row>
@@ -887,32 +893,33 @@
         <v>67</v>
       </c>
       <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294.8</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G9" s="2">
         <v>44811</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" s="1">
         <v>10</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>294.8</v>
       </c>
     </row>
@@ -927,32 +934,33 @@
         <v>66.5</v>
       </c>
       <c r="D10" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>292.60000000000002</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G10" s="2">
         <v>44812</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I10" s="1">
         <v>10</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>292.60000000000002</v>
       </c>
     </row>
@@ -967,32 +975,33 @@
         <v>66</v>
       </c>
       <c r="D11" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>290.40000000000003</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G11" s="2">
         <v>44813</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I11" s="1">
         <v>10</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>290.40000000000003</v>
       </c>
     </row>
@@ -1007,32 +1016,33 @@
         <v>65.5</v>
       </c>
       <c r="D12" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>288.20000000000005</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G12" s="2">
         <v>44814</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
         <v>10</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>298.20000000000005</v>
       </c>
     </row>
@@ -1047,32 +1057,33 @@
         <v>65</v>
       </c>
       <c r="D13" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>286</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G13" s="2">
         <v>44815</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I13" s="1">
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>306</v>
       </c>
     </row>
@@ -1087,32 +1098,33 @@
         <v>64.5</v>
       </c>
       <c r="D14" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283.8</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G14" s="2">
         <v>44816</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="I14" s="1">
         <v>10</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>313.8</v>
       </c>
     </row>
@@ -1127,32 +1139,33 @@
         <v>64</v>
       </c>
       <c r="D15" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281.60000000000002</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G15" s="2">
         <v>44817</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="I15" s="1">
         <v>10</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>321.60000000000002</v>
       </c>
     </row>
@@ -1167,32 +1180,33 @@
         <v>63.5</v>
       </c>
       <c r="D16" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279.40000000000003</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G16" s="2">
         <v>44818</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="I16" s="1">
         <v>10</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>329.40000000000003</v>
       </c>
     </row>
@@ -1207,32 +1221,33 @@
         <v>63</v>
       </c>
       <c r="D17" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>277.20000000000005</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G17" s="2">
         <v>44819</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="I17" s="1">
         <v>10</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>337.20000000000005</v>
       </c>
     </row>
@@ -1247,32 +1262,33 @@
         <v>62.5</v>
       </c>
       <c r="D18" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>275</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G18" s="2">
         <v>44820</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="I18" s="1">
         <v>10</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>345</v>
       </c>
     </row>
@@ -1287,32 +1303,33 @@
         <v>62</v>
       </c>
       <c r="D19" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>272.8</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G19" s="2">
         <v>44821</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="I19" s="1">
         <v>10</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>352.8</v>
       </c>
     </row>
@@ -1327,32 +1344,33 @@
         <v>61.5</v>
       </c>
       <c r="D20" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>270.60000000000002</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G20" s="2">
         <v>44822</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="I20" s="1">
         <v>10</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>360.6</v>
       </c>
     </row>
@@ -1367,32 +1385,33 @@
         <v>61</v>
       </c>
       <c r="D21" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>268.40000000000003</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G21" s="2">
         <v>44823</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I21" s="1">
         <v>10</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>368.40000000000003</v>
       </c>
     </row>
@@ -1407,14 +1426,15 @@
         <v>60.5</v>
       </c>
       <c r="D22" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>266.20000000000005</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G22" s="2">
@@ -1428,11 +1448,11 @@
         <v>10</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>376.20000000000005</v>
       </c>
     </row>
@@ -1447,32 +1467,33 @@
         <v>60</v>
       </c>
       <c r="D23" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>264</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G23" s="2">
         <v>44825</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="I23" s="1">
         <v>10</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>384</v>
       </c>
     </row>
@@ -1487,32 +1508,33 @@
         <v>59.5</v>
       </c>
       <c r="D24" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>261.8</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G24" s="2">
         <v>44826</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I24" s="1">
         <v>10</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>391.8</v>
       </c>
     </row>
@@ -1527,32 +1549,33 @@
         <v>59</v>
       </c>
       <c r="D25" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>259.60000000000002</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G25" s="2">
         <v>44827</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="I25" s="1">
         <v>10</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>399.6</v>
       </c>
     </row>
@@ -1567,32 +1590,33 @@
         <v>58.5</v>
       </c>
       <c r="D26" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>257.40000000000003</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G26" s="2">
         <v>44828</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="I26" s="1">
         <v>10</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>407.40000000000003</v>
       </c>
     </row>
@@ -1607,32 +1631,33 @@
         <v>58</v>
       </c>
       <c r="D27" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>255.20000000000002</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G27" s="2">
         <v>44829</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="I27" s="1">
         <v>10</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>415.20000000000005</v>
       </c>
     </row>
@@ -1647,32 +1672,33 @@
         <v>57.5</v>
       </c>
       <c r="D28" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>253.00000000000003</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G28" s="2">
         <v>44830</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="I28" s="1">
         <v>10</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>423</v>
       </c>
     </row>
@@ -1687,32 +1713,33 @@
         <v>57</v>
       </c>
       <c r="D29" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>250.8</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G29" s="2">
         <v>44831</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="I29" s="1">
         <v>10</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>430.8</v>
       </c>
     </row>
@@ -1727,32 +1754,33 @@
         <v>56.5</v>
       </c>
       <c r="D30" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>248.60000000000002</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G30" s="2">
         <v>44832</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="I30" s="1">
         <v>10</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>438.6</v>
       </c>
     </row>
@@ -1767,32 +1795,33 @@
         <v>56</v>
       </c>
       <c r="D31" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>246.40000000000003</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G31" s="2">
         <v>44833</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="I31" s="1">
         <v>10</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>446.40000000000003</v>
       </c>
     </row>
@@ -1807,32 +1836,33 @@
         <v>55.5</v>
       </c>
       <c r="D32" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>244.20000000000002</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G32" s="2">
         <v>44834</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="I32" s="1">
         <v>10</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>454.20000000000005</v>
       </c>
     </row>
@@ -1847,32 +1877,33 @@
         <v>55</v>
       </c>
       <c r="D33" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>242.00000000000003</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G33" s="2">
         <v>44835</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="I33" s="1">
         <v>10</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>462</v>
       </c>
     </row>
@@ -1887,32 +1918,33 @@
         <v>54.5</v>
       </c>
       <c r="D34" s="1">
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>239.8</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G34" s="2">
         <v>44836</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="I34" s="1">
         <v>10</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>230</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>469.8</v>
       </c>
     </row>
@@ -1927,32 +1959,33 @@
         <v>54</v>
       </c>
       <c r="D35" s="1">
+        <f>4*1.1/2</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>118.80000000000001</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G35" s="2">
         <v>44837</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="I35" s="1">
         <v>10</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>358.8</v>
       </c>
     </row>
@@ -1967,32 +2000,33 @@
         <v>53.5</v>
       </c>
       <c r="D36" s="1">
+        <f t="shared" ref="D36:D38" si="6">4*1.1/2</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>117.7</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G36" s="2">
         <v>44838</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="I36" s="1">
         <v>10</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="K36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>367.7</v>
       </c>
     </row>
@@ -2007,32 +2041,33 @@
         <v>53</v>
       </c>
       <c r="D37" s="1">
+        <f t="shared" si="6"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>116.60000000000001</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G37" s="2">
         <v>44839</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="I37" s="1">
         <v>10</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>260</v>
       </c>
       <c r="K37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>376.6</v>
       </c>
     </row>
@@ -2047,32 +2082,33 @@
         <v>52.5</v>
       </c>
       <c r="D38" s="1">
+        <f t="shared" si="6"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>115.50000000000001</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44813</v>
       </c>
       <c r="G38" s="2">
         <v>44840</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="I38" s="1">
         <v>10</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>270</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>385.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xdd 3 pop 3
</commit_message>
<xml_diff>
--- a/LR3/table_1_4.xlsx
+++ b/LR3/table_1_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E220C9BD-4A6D-4CE3-BB36-1A6B96F2936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5760396C-A2DC-4C82-987F-FC7E605759ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{C812E225-0302-43BC-BF7F-7687DCBD0107}"/>
+    <workbookView xWindow="3750" yWindow="2850" windowWidth="21600" windowHeight="11295" xr2:uid="{C812E225-0302-43BC-BF7F-7687DCBD0107}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>№ квартиры</t>
   </si>
   <si>
-    <t>Фамилия квартиросъемщика</t>
-  </si>
-  <si>
     <t>Абдуллина</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>Куропаткин 1</t>
   </si>
   <si>
-    <t>Купропаткин 2</t>
-  </si>
-  <si>
     <t>Срок оплаты</t>
   </si>
   <si>
@@ -188,6 +182,12 @@
   </si>
   <si>
     <t>Максимальная сумма к оплате, руб.</t>
+  </si>
+  <si>
+    <t>Куропаткин 2</t>
+  </si>
+  <si>
+    <t>Фамилия квартиросъёмщика</t>
   </si>
 </sst>
 </file>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F7733E-DEB9-4F9D-8946-67364D2E8DA5}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,34 +614,34 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>69.5</v>
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>69</v>
@@ -775,7 +775,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>68.5</v>
@@ -817,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>68</v>
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>67.5</v>
@@ -901,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>67</v>
@@ -943,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>66.5</v>
@@ -985,7 +985,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
         <v>66</v>
@@ -1027,7 +1027,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
         <v>65.5</v>
@@ -1069,7 +1069,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>65</v>
@@ -1111,7 +1111,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>64.5</v>
@@ -1153,7 +1153,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="1">
         <v>64</v>
@@ -1195,7 +1195,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1">
         <v>63.5</v>
@@ -1237,7 +1237,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>63</v>
@@ -1279,7 +1279,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>62.5</v>
@@ -1321,7 +1321,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1">
         <v>62</v>
@@ -1363,7 +1363,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
         <v>61.5</v>
@@ -1405,7 +1405,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1">
         <v>61</v>
@@ -1447,7 +1447,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>60.5</v>
@@ -1489,7 +1489,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
         <v>60</v>
@@ -1531,7 +1531,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
         <v>59.5</v>
@@ -1573,7 +1573,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1">
         <v>59</v>
@@ -1615,7 +1615,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
         <v>58.5</v>
@@ -1657,7 +1657,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="1">
         <v>58</v>
@@ -1699,7 +1699,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1">
         <v>57.5</v>
@@ -1741,7 +1741,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
         <v>57</v>
@@ -1783,7 +1783,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="1">
         <v>56.5</v>
@@ -1825,7 +1825,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="1">
         <v>56</v>
@@ -1867,7 +1867,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="1">
         <v>55.5</v>
@@ -1909,7 +1909,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1">
         <v>55</v>
@@ -1951,7 +1951,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1">
         <v>54.5</v>
@@ -1993,7 +1993,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="1">
         <v>54</v>
@@ -2035,7 +2035,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="1">
         <v>53.5</v>
@@ -2077,7 +2077,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1">
         <v>53</v>
@@ -2119,7 +2119,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1">
         <v>52.5</v>
@@ -2171,7 +2171,7 @@
     <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C40" s="3">
         <f>SUM(K3:K38)</f>
@@ -2189,7 +2189,7 @@
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1">
         <f>AVERAGE(C3:C38)</f>
@@ -2207,7 +2207,7 @@
     <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1">
         <f>MAX(H3:H38)</f>
@@ -2225,7 +2225,7 @@
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1">
         <f>MAX(E3:E38)</f>

</xml_diff>